<commit_message>
Add 2020.05.24 report of web data mining 1 group.
</commit_message>
<xml_diff>
--- a/读书报告分组提交/web data mining新组1/05.17讨论后的读书报告/2020.05.17读书报告汇总.xlsx
+++ b/读书报告分组提交/web data mining新组1/05.17讨论后的读书报告/2020.05.17读书报告汇总.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pycharm_home\Reading-Club\读书报告分组提交\web data mining新组1\05.17讨论后的读书报告\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEE5152-8B02-4F37-AA6A-6921976FCE11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A83979B-31E2-4D28-BC08-C316880EC4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>成员</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -210,12 +210,23 @@
       <t>章</t>
     </r>
   </si>
+  <si>
+    <t>李泓烨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看完第12章</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +265,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -275,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -318,6 +337,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -598,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -621,53 +647,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12" t="s">
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="31.2" customHeight="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13" t="s">
+      <c r="G2" s="16"/>
+      <c r="H2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13" t="s">
+      <c r="I2" s="16"/>
+      <c r="J2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="12"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:12" ht="28.8" customHeight="1">
-      <c r="A3" s="12"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
@@ -698,7 +724,7 @@
       <c r="K3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="12"/>
+      <c r="L3" s="17"/>
     </row>
     <row r="4" spans="1:12" ht="15">
       <c r="A4" s="1" t="s">
@@ -711,7 +737,9 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3">
+        <v>30</v>
+      </c>
       <c r="F4" s="14" t="s">
         <v>27</v>
       </c>
@@ -732,7 +760,7 @@
       </c>
       <c r="L4" s="4">
         <f>SUM(C4,E4,G4,I4,K4)</f>
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.4">
@@ -748,6 +776,9 @@
       <c r="D5" s="1">
         <v>2</v>
       </c>
+      <c r="E5" s="1">
+        <v>35</v>
+      </c>
       <c r="F5" s="15" t="s">
         <v>29</v>
       </c>
@@ -768,7 +799,7 @@
       </c>
       <c r="L5" s="7">
         <f>SUM(C5,E5,G5,I5,K5)</f>
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="27.6">
@@ -782,6 +813,9 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
+      <c r="E6" s="1">
+        <v>30</v>
+      </c>
       <c r="F6" s="15" t="s">
         <v>34</v>
       </c>
@@ -802,7 +836,7 @@
       </c>
       <c r="L6" s="7">
         <f>SUM(C6,E6,G6,I6,K6)</f>
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="14.4">
@@ -824,75 +858,105 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="27.6">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:12" s="12" customFormat="1">
+      <c r="A8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0</v>
+      </c>
+      <c r="D8" s="12">
+        <v>2</v>
+      </c>
+      <c r="E8" s="12">
+        <v>35</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="12">
+        <v>15</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <v>6</v>
+      </c>
+      <c r="L8" s="12">
+        <f>SUM(C8,E8,G8,I8,K8)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="27.6">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
         <v>0</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C9" s="6">
         <v>28</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <v>2</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="15" t="s">
+      <c r="E9" s="3">
+        <v>30</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G9" s="7">
         <v>15</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I9" s="4">
         <v>4</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K9" s="11">
         <v>6</v>
       </c>
-      <c r="L8" s="7">
-        <f>SUM(C8,E8,G8,I8,K8)</f>
-        <v>53</v>
+      <c r="L9" s="7">
+        <f>SUM(C9,E9,G9,I9,K9)</f>
+        <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="27.6" customHeight="1">
-      <c r="B9" s="13" t="s">
+    <row r="10" spans="1:12" ht="27.6" customHeight="1">
+      <c r="B10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13" t="s">
+      <c r="E10" s="16"/>
+      <c r="F10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13" t="s">
+      <c r="G10" s="16"/>
+      <c r="H10" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13" t="s">
+      <c r="I10" s="16"/>
+      <c r="J10" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="13"/>
+      <c r="K10" s="16"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L8">
-    <sortCondition descending="1" ref="L8"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L9">
+    <sortCondition descending="1" ref="L9"/>
   </sortState>
   <mergeCells count="14">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
     <mergeCell ref="L1:L3"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A1:A3"/>
@@ -902,6 +966,11 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="H1:K1"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add 2020.05.31 folder of web data mining 1 group.
</commit_message>
<xml_diff>
--- a/读书报告分组提交/web data mining新组1/05.17讨论后的读书报告/2020.05.17读书报告汇总.xlsx
+++ b/读书报告分组提交/web data mining新组1/05.17讨论后的读书报告/2020.05.17读书报告汇总.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pycharm_home\Reading-Club\读书报告分组提交\web data mining新组1\05.17讨论后的读书报告\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A83979B-31E2-4D28-BC08-C316880EC4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7492392-F783-4E45-8816-FAD24588A29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,10 +74,6 @@
   </si>
   <si>
     <t>方骏</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>喻泽弘</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -220,6 +216,10 @@
   </si>
   <si>
     <t>看完第12章</t>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -309,9 +309,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -319,9 +316,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -344,6 +338,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -624,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -651,7 +651,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
@@ -659,7 +659,7 @@
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
       <c r="H1" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" s="17"/>
       <c r="J1" s="17"/>
@@ -670,293 +670,289 @@
     </row>
     <row r="2" spans="1:12" ht="31.2" customHeight="1">
       <c r="A2" s="17"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="16"/>
+      <c r="K2" s="18"/>
       <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:12" ht="28.8" customHeight="1">
       <c r="A3" s="17"/>
       <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="K3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="L3" s="17"/>
     </row>
-    <row r="4" spans="1:12" ht="15">
+    <row r="4" spans="1:12" ht="27.6">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="5">
+        <v>40</v>
+      </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="3">
         <v>30</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="5">
+        <v>15</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="6">
-        <v>15</v>
-      </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="14">
+        <v>4</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="6">
-        <v>3</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>6</v>
       </c>
       <c r="L4" s="4">
         <f>SUM(C4,E4,G4,I4,K4)</f>
-        <v>54</v>
+        <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.4">
+    <row r="5" spans="1:12" ht="15">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>40</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>35</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="7">
+        <v>30</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="6">
         <v>15</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I5" s="4">
         <v>3</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="9">
+        <v>6</v>
+      </c>
+      <c r="L5" s="6">
+        <f>SUM(C5,E5,G5,I5,K5)</f>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="14.4">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>35</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="6">
+        <v>15</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="15">
+        <v>3</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="9">
+        <v>6</v>
+      </c>
+      <c r="L6" s="6">
+        <f>SUM(C6,E6,G6,I6,K6)</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="10" customFormat="1">
+      <c r="A7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10">
+        <v>28</v>
+      </c>
+      <c r="D7" s="10">
+        <v>2</v>
+      </c>
+      <c r="E7" s="10">
+        <v>35</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="10">
+        <v>15</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="10">
+        <v>6</v>
+      </c>
+      <c r="L7" s="10">
+        <f>SUM(C7,E7,G7,I7,K7)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="27.6">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>30</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="11">
+      <c r="G8" s="6">
+        <v>15</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="4">
+        <v>4</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="9">
         <v>6</v>
       </c>
-      <c r="L5" s="7">
-        <f>SUM(C5,E5,G5,I5,K5)</f>
-        <v>87</v>
+      <c r="L8" s="6">
+        <f>SUM(C8,E8,G8,I8,K8)</f>
+        <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="27.6">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>30</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="7">
-        <v>15</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="9">
-        <v>4</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="11">
-        <v>6</v>
-      </c>
-      <c r="L6" s="7">
-        <f>SUM(C6,E6,G6,I6,K6)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="14.4">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="11">
-        <v>6</v>
-      </c>
-      <c r="L7" s="7">
-        <f>SUM(C7,E7,G7,I7,K7)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="12" customFormat="1">
-      <c r="A8" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="12">
-        <v>0</v>
-      </c>
-      <c r="D8" s="12">
-        <v>2</v>
-      </c>
-      <c r="E8" s="12">
-        <v>35</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="12">
-        <v>15</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="12">
-        <v>0</v>
-      </c>
-      <c r="K8" s="12">
-        <v>6</v>
-      </c>
-      <c r="L8" s="12">
-        <f>SUM(C8,E8,G8,I8,K8)</f>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="27.6">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="6">
-        <v>28</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3">
-        <v>30</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="7">
-        <v>15</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="4">
-        <v>4</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" s="11">
-        <v>6</v>
-      </c>
-      <c r="L9" s="7">
-        <f>SUM(C9,E9,G9,I9,K9)</f>
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="27.6" customHeight="1">
-      <c r="B10" s="16" t="s">
+    <row r="9" spans="1:12" ht="27.6" customHeight="1">
+      <c r="B9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16" t="s">
+      <c r="E9" s="18"/>
+      <c r="F9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16" t="s">
+      <c r="G9" s="18"/>
+      <c r="H9" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16" t="s">
+      <c r="I9" s="18"/>
+      <c r="J9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="K10" s="16"/>
+      <c r="K9" s="18"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L9">
-    <sortCondition descending="1" ref="L9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L8">
+    <sortCondition descending="1" ref="L8"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
     <mergeCell ref="L1:L3"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A1:A3"/>
@@ -966,11 +962,6 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="H1:K1"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>